<commit_message>
gain resistor R8 to 10k
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -92,9 +92,6 @@
     <t>zener</t>
   </si>
   <si>
-    <t>R8</t>
-  </si>
-  <si>
     <t>R9</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>R1-R2</t>
   </si>
   <si>
-    <t>R3-R6</t>
-  </si>
-  <si>
     <t>78-BZT55C9V1</t>
   </si>
   <si>
@@ -285,6 +279,12 @@
   </si>
   <si>
     <t>Rundrohr Alu eloxiert 12x1</t>
+  </si>
+  <si>
+    <t>R4, R8</t>
+  </si>
+  <si>
+    <t>R3, R5-R6</t>
   </si>
 </sst>
 </file>
@@ -802,7 +802,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,12 +823,12 @@
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -866,21 +866,21 @@
         <v>6</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="K4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="24"/>
       <c r="C5" s="24"/>
@@ -895,21 +895,21 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
       <c r="D6" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="18" t="s">
         <v>45</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>46</v>
       </c>
       <c r="H6" s="9">
         <v>0.62</v>
@@ -928,17 +928,17 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>7</v>
@@ -967,13 +967,13 @@
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="18" t="s">
         <v>7</v>
@@ -998,25 +998,25 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="F9" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="18" t="s">
         <v>47</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>48</v>
       </c>
       <c r="H9" s="9">
         <v>0.16400000000000001</v>
@@ -1044,16 +1044,16 @@
         <v>1206</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H10" s="9">
         <v>0.16200000000000001</v>
@@ -1075,22 +1075,22 @@
         <v>11</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="18">
         <v>1206</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H11" s="9">
         <v>0.09</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>16</v>
@@ -1118,16 +1118,16 @@
         <v>1206</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H12" s="9">
         <v>7.4999999999999997E-2</v>
@@ -1155,16 +1155,16 @@
         <v>19</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>20</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H13" s="9">
         <v>0.16500000000000001</v>
@@ -1183,23 +1183,23 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="18">
         <v>1206</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H14" s="9">
         <v>1.2999999999999999E-2</v>
@@ -1218,23 +1218,23 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="18">
         <v>1206</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H15" s="9">
         <v>2.5999999999999999E-2</v>
@@ -1253,23 +1253,23 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="18">
         <v>1206</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H16" s="9">
         <v>1.2999999999999999E-2</v>
@@ -1288,7 +1288,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="18">
         <v>220</v>
@@ -1298,13 +1298,13 @@
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H17" s="9">
         <v>3.2000000000000001E-2</v>
@@ -1323,23 +1323,23 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="18">
         <v>1206</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H18" s="9">
         <v>1.7999999999999999E-2</v>
@@ -1358,7 +1358,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B19" s="18">
         <v>100</v>
@@ -1368,13 +1368,13 @@
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H19" s="9">
         <v>1.4999999999999999E-2</v>
@@ -1396,13 +1396,13 @@
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
       <c r="D20" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G20" s="18">
         <v>160823</v>
@@ -1427,13 +1427,13 @@
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
       <c r="D21" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>35</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>36</v>
       </c>
       <c r="G21" s="18">
         <v>182696</v>
@@ -1455,7 +1455,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
@@ -1473,13 +1473,13 @@
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G23" s="18">
         <v>6449190</v>
@@ -1505,10 +1505,10 @@
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G24" s="18"/>
       <c r="H24" s="9">
@@ -1531,13 +1531,13 @@
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="18" t="s">
-        <v>42</v>
-      </c>
       <c r="F25" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G25" s="18">
         <v>1571483</v>
@@ -1563,10 +1563,10 @@
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
@@ -1590,10 +1590,10 @@
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
       <c r="D27" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="18" t="s">
         <v>78</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>80</v>
       </c>
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
@@ -1617,10 +1617,10 @@
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
       <c r="D28" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>

</xml_diff>